<commit_message>
Co-authored-by: youngaoumaima <youngaoumaima@users.noreply.github.com> Co-authored-by: InfoPr <InfoPr@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/oumaima.xlsx
+++ b/oumaima.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+  <si>
+    <t/>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -82,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +96,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -124,28 +133,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,197 +461,226 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="34.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="34.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="4">
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1"/>
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1"/>
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6">
+        <v>77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1"/>
+      <c r="B7" s="6">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6">
         <v>7</v>
       </c>
-      <c r="D3" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="1"/>
+      <c r="B13" s="6">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4">
-        <v>77</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="4">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="D6" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="4">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="4">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="4">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="4">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="4">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="4">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="E14" s="4">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Co-authored-by: youngaoumaima <youngaoumaima@users.noreply.github.com> Co-authored-by: rania.fe06@gmail.com <rania.fe06@gmail.com> Co-authored-by: InfoPr <InfoPr@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/oumaima.xlsx
+++ b/oumaima.xlsx
@@ -15,69 +15,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>has_more_than_</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>ahmed@ghldsk.dkg</t>
+  </si>
+  <si>
+    <t>medea, avenue 5|medea, avenue6</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>mostapha</t>
+  </si>
+  <si>
+    <t>mostapha@ghldsk.dkg</t>
+  </si>
+  <si>
+    <t>chlef, kldfjdskl street 19</t>
+  </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>ahmed</t>
-  </si>
-  <si>
-    <t>ahmed@ghldsk.dkg</t>
-  </si>
-  <si>
-    <t>mostapha</t>
-  </si>
-  <si>
-    <t>mostapha@ghldsk.dkg</t>
-  </si>
-  <si>
     <t>ooyy</t>
   </si>
   <si>
     <t>youngaoumaima@gmail.com</t>
   </si>
   <si>
+    <t>paris, slkdfkl 2</t>
+  </si>
+  <si>
     <t>gf</t>
   </si>
   <si>
     <t>bryyoungabenaissa@gmail.com</t>
   </si>
   <si>
+    <t>medea, route d'alger</t>
+  </si>
+  <si>
     <t>mostapha1@ghldsk.dkg</t>
   </si>
   <si>
+    <t>medea, beziouch</t>
+  </si>
+  <si>
     <t>rania</t>
   </si>
   <si>
+    <t>klsdjfjkl@lsdjk.com</t>
+  </si>
+  <si>
+    <t>chlef, algeria</t>
+  </si>
+  <si>
+    <t>rania1</t>
+  </si>
+  <si>
+    <t>dsflksdjf.dsfkldsjfs@fklsdj</t>
+  </si>
+  <si>
+    <t>paris, france</t>
+  </si>
+  <si>
+    <t>roeoe1</t>
+  </si>
+  <si>
+    <t>rania.fe061@gmail.com</t>
+  </si>
+  <si>
+    <t>medea,algeria</t>
+  </si>
+  <si>
+    <t>zahia</t>
+  </si>
+  <si>
     <t>rania.fe06@gmail.com</t>
   </si>
   <si>
-    <t>zahia</t>
-  </si>
-  <si>
     <t>ahmed12@ghldsk.dkg</t>
   </si>
   <si>
+    <t>nice, france</t>
+  </si>
+  <si>
     <t>ahm3456@ghldsk.dkg</t>
   </si>
   <si>
+    <t>null</t>
+  </si>
+  <si>
     <t>dslkfjds</t>
   </si>
   <si>
     <t>lsdkjfdskl@llksdgj.com</t>
+  </si>
+  <si>
+    <t>fjd</t>
+  </si>
+  <si>
+    <t>skldjfklds@wlksfjdsl.clsdj</t>
+  </si>
+  <si>
+    <t>london, uk</t>
   </si>
 </sst>
 </file>
@@ -95,13 +158,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -133,15 +196,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -149,6 +206,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -461,227 +521,343 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="34.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="52.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2">
         <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2">
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21.75">
       <c r="A5" s="1"/>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6">
-        <v>77</v>
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5">
+        <v>78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1"/>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2">
         <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="6">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="6">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="6">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
-      <c r="B11" s="6">
+      <c r="B11" s="2">
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="6">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="6">
+      <c r="B12" s="2">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="6">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1"/>
-      <c r="B13" s="6">
-        <v>8</v>
+      <c r="B13" s="2">
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="6">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
-      <c r="B14" s="6">
+      <c r="B14" s="2">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2">
         <v>20</v>
       </c>
-      <c r="E14" s="4">
-        <v>12</v>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>